<commit_message>
Upload added Converted sms and email to functions
</commit_message>
<xml_diff>
--- a/workbooks/StudentDetails.xlsx
+++ b/workbooks/StudentDetails.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>roll_no</t>
   </si>
@@ -38,22 +38,25 @@
     <t>mobile</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>ab@gf</t>
-  </si>
-  <si>
-    <t>chdnb@tnv</t>
-  </si>
-  <si>
-    <t>fdjkfd@kogfjg</t>
+    <t>Arun Nair</t>
+  </si>
+  <si>
+    <t>appuarunnair@gmail.com</t>
+  </si>
+  <si>
+    <t>Aditya Kurhade</t>
+  </si>
+  <si>
+    <t>adikrhd@gmail.com</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>CSH14030</t>
+  </si>
+  <si>
+    <t>CSH14038</t>
   </si>
 </sst>
 </file>
@@ -77,12 +80,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,10 +109,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -385,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,67 +407,64 @@
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>312312312</v>
+        <v>9820055038</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>31231234</v>
+        <v>9664240554</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>546646</v>
-      </c>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>